<commit_message>
fixed getRow methods to parse cell position correctly
</commit_message>
<xml_diff>
--- a/src/test/resources/small-excel.xlsx
+++ b/src/test/resources/small-excel.xlsx
@@ -333,15 +333,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>CONCATENATE("HEADER - ", SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""))</f>
         <v>HEADER - A</v>
@@ -363,7 +363,7 @@
         <v>HEADER - E</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
         <v>A2</v>
@@ -385,7 +385,7 @@
         <v>E2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="2">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
         <v>A3</v>
@@ -406,8 +406,12 @@
         <f t="shared" si="1"/>
         <v>E3</v>
       </c>
+      <c r="AA3" t="str">
+        <f t="shared" ref="AA3" si="3">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>AA3</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="2"/>
         <v>A4</v>
@@ -429,7 +433,7 @@
         <v>E4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="2"/>
         <v>A5</v>

</xml_diff>

<commit_message>
Persist excel data to db with single and mutlithreaded options
</commit_message>
<xml_diff>
--- a/src/test/resources/small-excel.xlsx
+++ b/src/test/resources/small-excel.xlsx
@@ -333,15 +333,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>CONCATENATE("HEADER - ", SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""))</f>
         <v>HEADER - A</v>
@@ -363,7 +363,7 @@
         <v>HEADER - E</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
         <v>A2</v>
@@ -385,7 +385,7 @@
         <v>E2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="2">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
         <v>A3</v>
@@ -406,12 +406,8 @@
         <f t="shared" si="1"/>
         <v>E3</v>
       </c>
-      <c r="AA3" t="str">
-        <f t="shared" ref="AA3" si="3">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
-        <v>AA3</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="2"/>
         <v>A4</v>
@@ -433,7 +429,7 @@
         <v>E4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="2"/>
         <v>A5</v>

</xml_diff>